<commit_message>
ver pregunta terminado, responder hasta la carga de valores
</commit_message>
<xml_diff>
--- a/CarreraObsGenerador.xlsx
+++ b/CarreraObsGenerador.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\drive\CarreraObservacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\C_Obs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Carrera" sheetId="1" r:id="rId1"/>
@@ -27,41 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>estado</t>
-  </si>
-  <si>
-    <t>nombres</t>
-  </si>
-  <si>
-    <t>apellidos</t>
-  </si>
-  <si>
     <t>color</t>
   </si>
   <si>
-    <t>pista</t>
-  </si>
-  <si>
-    <t>carreraId</t>
-  </si>
-  <si>
-    <t>codigo</t>
-  </si>
-  <si>
-    <t>respuesta</t>
-  </si>
-  <si>
-    <t>nodoId</t>
-  </si>
-  <si>
     <t>COSem12016</t>
   </si>
   <si>
@@ -95,9 +68,6 @@
     <t>SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR</t>
   </si>
   <si>
-    <t>www.autonoma.edu.co/biblioteca</t>
-  </si>
-  <si>
     <t>EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS</t>
   </si>
   <si>
@@ -197,9 +167,6 @@
     <t>ALLI EJERCICIO, JUGAR Y LIBERAR TENSION PUEDES REALIZAR</t>
   </si>
   <si>
-    <t>UNA FORMA DIFERENTE DE COMUNICARTE ALLI APRENDERAS</t>
-  </si>
-  <si>
     <t>OLVIDO DE CONTRASEÑAS Y PROBLEMAS DE INGRESO A LOS SISTEMAS AQUÍ TE SOLUCIONARAN</t>
   </si>
   <si>
@@ -212,51 +179,6 @@
     <t>LAS HERRAMIENTAS COMPUTACIONES EN ESTE PISO ENTERO ENCONTRARAS</t>
   </si>
   <si>
-    <t>www.autonoma.edu.co/caja</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/registro_academico</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/mercadeo</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/relaciones_internacionales</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/cartera</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/desarrollo_humano</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/servicios_medicos</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/atencion_prehospitalaria</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/laboratorio_electronica</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/gimnasio</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/laboratorio_de_ingles</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/gestion_de_tecnologia</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/decanatura_ingenieria</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/sala_de_profesores_de_ingenieria</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/centro_de_informatica</t>
-  </si>
-  <si>
     <t>¿CUÁL ES EL NOMBRE DE LA SALA DONDE VIDEOS Y PELÍCULAS PUEDES ENCONTRAR?</t>
   </si>
   <si>
@@ -332,27 +254,12 @@
     <t>GABRIEL CADENA GOMEZ</t>
   </si>
   <si>
-    <t>VICERRECTORIA ADMINISTRATIVA</t>
-  </si>
-  <si>
     <t>CUANDO PROBLEMAS ACADÉMICOS ENCUENTRES, ESTE ES EL MÁXIMO ESTAMENTO A CONSULTAR</t>
   </si>
   <si>
     <t>DESDE ALLÍ SE DIRIGE LA UAM</t>
   </si>
   <si>
-    <t>www.autonoma.edu.co/rectoria</t>
-  </si>
-  <si>
-    <t>www.autonoma.edu.co/vicerrectoria_academica</t>
-  </si>
-  <si>
-    <t>¿NOMBRA AL VICERRECTOR ADMINISTRATIVO DE LA UAM?</t>
-  </si>
-  <si>
-    <t>CARLOS EDUARDO JARAMILLO SANINT</t>
-  </si>
-  <si>
     <t>¿ELLA ES LA ENCARGADA DE ASIGNARTE CITAS Y RECIBIRTE EN ESTE LUGAR?</t>
   </si>
   <si>
@@ -416,24 +323,9 @@
     <t>MARTHA LILIA MORALES GONZALEZ</t>
   </si>
   <si>
-    <t>descripcion</t>
-  </si>
-  <si>
     <t>Primera carrera de observación</t>
   </si>
   <si>
-    <t>fecha nacimiento</t>
-  </si>
-  <si>
-    <t>mail</t>
-  </si>
-  <si>
-    <t>genero</t>
-  </si>
-  <si>
-    <t>tipo</t>
-  </si>
-  <si>
     <t>hombre</t>
   </si>
   <si>
@@ -449,19 +341,73 @@
     <t>14/04/1978</t>
   </si>
   <si>
-    <t>ubicación</t>
-  </si>
-  <si>
-    <t>20,120</t>
-  </si>
-  <si>
     <t>¿CUÁL ES EL CORRE DE ATENCIÓN GENERAL DE ESTE LUGAR?</t>
   </si>
   <si>
     <t>GESTEC@AUTONOMA.EDU.CO</t>
   </si>
   <si>
-    <t>enunciado</t>
+    <t>name</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>birthDate</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Intersemestral2016</t>
+  </si>
+  <si>
+    <t>carrera de observacion intersemestral</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>RAND()</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>hint</t>
+  </si>
+  <si>
+    <t>circuit_id</t>
+  </si>
+  <si>
+    <t>question</t>
+  </si>
+  <si>
+    <t>answer</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>20.1</t>
+  </si>
+  <si>
+    <t>120.5</t>
   </si>
 </sst>
 </file>
@@ -793,10 +739,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,6 +750,7 @@
     <col min="1" max="1" width="9.85546875" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="15.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -812,13 +759,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -826,17 +773,35 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>98</v>
       </c>
       <c r="E2" t="str">
-        <f>CONCATENATE("INSERT  INTO carrera (nombre, estado, descripcion) VALUES ('",B2,"', ",C2,",'",D2, "');")</f>
-        <v>INSERT  INTO carrera (nombre, estado, descripcion) VALUES ('COSem12016', 1,'Primera carrera de observación');</v>
+        <f>CONCATENATE("INSERT  INTO circuit (name, status, description) VALUES ('",B2,"', ",C2,",'",D2, "');")</f>
+        <v>INSERT  INTO circuit (name, status, description) VALUES ('COSem12016', 1,'Primera carrera de observación');</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" t="str">
+        <f>CONCATENATE("INSERT  INTO circuit (name, status, description) VALUES ('",B3,"', ",C3,",'",D3, "');")</f>
+        <v>INSERT  INTO circuit (name, status, description) VALUES ('Intersemestral2016', 1,'carrera de observacion intersemestral');</v>
       </c>
     </row>
   </sheetData>
@@ -848,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -870,25 +835,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="E1" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G1" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="H1" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,29 +861,29 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>138</v>
+        <v>102</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="G2" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="H2" t="s">
-        <v>136</v>
+        <v>100</v>
       </c>
       <c r="I2" t="str">
-        <f>CONCATENATE("INSERT  INTO usuario (nombres, apellidos, fechaNacimiento, mail, color, genero, tipo) VALUES (","'",B2, "', '",C2,"', '",D2, "', '",E2,"', '",F2, "', '",G2,"','",H2,"');")</f>
-        <v>INSERT  INTO usuario (nombres, apellidos, fechaNacimiento, mail, color, genero, tipo) VALUES ('JULIAN MAURICIO', 'MEJIA CARDONA', '28/01/1984', 'jmmejia@autonoma.edu.co', 'verde', 'hombre','administrador');</v>
+        <f>CONCATENATE("INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES (","'",B2, "', '",C2,"', '",D2, "', '",E2,"', '",F2, "', '",G2,"','",H2,"');")</f>
+        <v>INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES ('JULIAN MAURICIO', 'MEJIA CARDONA', '28/01/1984', 'jmmejia@autonoma.edu.co', 'verde', 'hombre','administrador');</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -926,29 +891,29 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>139</v>
+        <v>103</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="H3" t="s">
-        <v>137</v>
+        <v>101</v>
       </c>
       <c r="I3" t="str">
-        <f>CONCATENATE("INSERT  INTO usuario (nombres, apellidos, fechaNacimiento, mail, color, genero, tipo) VALUES (","'",B3, "', '",C3,"', '",D3, "', '",E3,"', '",F3, "', '",G3,"','",H3,"');")</f>
-        <v>INSERT  INTO usuario (nombres, apellidos, fechaNacimiento, mail, color, genero, tipo) VALUES ('JORGE IVAN', 'MEZA MARTINEZ', '14/04/1978', 'jimezam@autonoma.edu.co', 'azul', 'hombre','usuario');</v>
+        <f>CONCATENATE("INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES (","'",B3, "', '",C3,"', '",D3, "', '",E3,"', '",F3, "', '",G3,"','",H3,"');")</f>
+        <v>INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES ('JORGE IVAN', 'MEZA MARTINEZ', '14/04/1978', 'jimezam@autonoma.edu.co', 'azul', 'hombre','usuario');</v>
       </c>
     </row>
   </sheetData>
@@ -963,10 +928,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I21" sqref="I2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,540 +939,659 @@
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="111.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="111.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="F1" t="s">
-        <v>6</v>
+        <v>119</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="H1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>117</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2" t="str">
-        <f>CONCATENATE("INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES (", " '",B2,"', '",C2, "', '",D2,"', '",E2,"', '",F2, "', ",G2,");")</f>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', 'www.autonoma.edu.co/biblioteca', '20,120', 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="str">
+        <f>CONCATENATE("INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES (", " '",B2,"', '",C2, "', ",D2,", ",E2,", ",F2, ", '",G2,"', ",H2,");")</f>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 20.1, 120.5, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D3" t="s">
-        <v>61</v>
+        <v>24</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F3" t="s">
-        <v>47</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3" t="str">
-        <f t="shared" ref="H3:H19" si="0">CONCATENATE("INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES (", " '",B3,"', '",C3, "', '",D3,"', '",E3,"', '",F3, "', ",G3,");")</f>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'CAJA', 'CAJA', 'www.autonoma.edu.co/caja', '20,120', 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 1);</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I21" si="0">CONCATENATE("INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES (", " '",B3,"', '",C3, "', ",D3,", ",E3,", ",F3, ", '",G3,"', ",H3,");")</f>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 20.1, 120.5, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 1);</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
+        <v>33</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', 'www.autonoma.edu.co/registro_academico', '20,120', 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 1);</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 20.1, 120.5, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 1);</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>63</v>
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'MERCADEO', 'MERCADEO', 'www.autonoma.edu.co/mercadeo', '20,120', 'SUS ENCARGADOS LA OFERTA ACADEMICA Y AYUDA ADMINISTRATIVA TE OFRECERAN', 1);</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'MERCADEO', 'MERCADEO', RAND(), 20.1, 120.5, 'SUS ENCARGADOS LA OFERTA ACADEMICA Y AYUDA ADMINISTRATIVA TE OFRECERAN', 1);</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6">
-        <v>1</v>
-      </c>
-      <c r="H6" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'RELACIONES INTERNACIONALES', 'RELACIONES INTERNACIONALES', 'www.autonoma.edu.co/relaciones_internacionales', '20,120', 'SI UN INTERCAMBIO QUIERES HACER A ESTE LUGAR DEBES LLEGAR', 1);</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RELACIONES INTERNACIONALES', 'RELACIONES INTERNACIONALES', RAND(), 20.1, 120.5, 'SI UN INTERCAMBIO QUIERES HACER A ESTE LUGAR DEBES LLEGAR', 1);</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>65</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'CARTERA', 'CARTERA', 'www.autonoma.edu.co/cartera', '20,120', 'PLAZOS DE FINANCIAMIENTO Y OPCIONES A PROBLEMAS ECONOMICAS ACA TE DARAN', 1);</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G7" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CARTERA', 'CARTERA', RAND(), 20.1, 120.5, 'PLAZOS DE FINANCIAMIENTO Y OPCIONES A PROBLEMAS ECONOMICAS ACA TE DARAN', 1);</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
+        <v>27</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'DESARROLLO HUMANO', 'DESARROLLO HUMANO', 'www.autonoma.edu.co/desarrollo_humano', '20,120', 'SUS ENCARGADOS VELAN POR TU BIENESTAR MENTAL Y PSICOLOGICO, ADEMAS DE AYUDA CON DIFICULTADES ACADEMICAS', 1);</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DESARROLLO HUMANO', 'DESARROLLO HUMANO', RAND(), 20.1, 120.5, 'SUS ENCARGADOS VELAN POR TU BIENESTAR MENTAL Y PSICOLOGICO, ADEMAS DE AYUDA CON DIFICULTADES ACADEMICAS', 1);</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>67</v>
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'SERVICIOS MEDICOS', 'SERVICIOS MEDICOS', 'www.autonoma.edu.co/servicios_medicos', '20,120', 'EN ESTE SITIO ENCONTRARAS UN MEDICO QUE TE PUEDE INDICAR QUE TRATAMIENTO TOMAR', 1);</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SERVICIOS MEDICOS', 'SERVICIOS MEDICOS', RAND(), 20.1, 120.5, 'EN ESTE SITIO ENCONTRARAS UN MEDICO QUE TE PUEDE INDICAR QUE TRATAMIENTO TOMAR', 1);</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>68</v>
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F10" t="s">
-        <v>54</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'ATENCION PREHOSPITALARIA', 'ATENCION PREHOSPITALARIA', 'www.autonoma.edu.co/atencion_prehospitalaria', '20,120', 'SI TE SIENTES FISICAMENTE MAL EN ESTE LUGAR UNA PERSONA PROFESIONAL TE ATENDERA', 1);</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'ATENCION PREHOSPITALARIA', 'ATENCION PREHOSPITALARIA', RAND(), 20.1, 120.5, 'SI TE SIENTES FISICAMENTE MAL EN ESTE LUGAR UNA PERSONA PROFESIONAL TE ATENDERA', 1);</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" t="s">
-        <v>69</v>
+        <v>30</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'LABORATORIO ELECTRONICA', 'LABORATORIO ELECTRONICA', 'www.autonoma.edu.co/laboratorio_electronica', '20,120', 'LOS MONTAJES ELECTRONICOS Y EXPERIMENTOS FISICOS EN ESTE LUGAR DESARROLLARAS', 1);</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'LABORATORIO ELECTRONICA', 'LABORATORIO ELECTRONICA', RAND(), 20.1, 120.5, 'LOS MONTAJES ELECTRONICOS Y EXPERIMENTOS FISICOS EN ESTE LUGAR DESARROLLARAS', 1);</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" t="s">
-        <v>70</v>
+        <v>29</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'GIMNASIO', 'GIMNASIO', 'www.autonoma.edu.co/gimnasio', '20,120', 'ALLI EJERCICIO, JUGAR Y LIBERAR TENSION PUEDES REALIZAR', 1);</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GIMNASIO', 'GIMNASIO', RAND(), 20.1, 120.5, 'ALLI EJERCICIO, JUGAR Y LIBERAR TENSION PUEDES REALIZAR', 1);</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" t="s">
-        <v>71</v>
+        <v>22</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'GESTION DE TECNOLOGIA', 'GESTION DE TECNOLOGIA', 'www.autonoma.edu.co/laboratorio_de_ingles', '20,120', 'UNA FORMA DIFERENTE DE COMUNICARTE ALLI APRENDERAS', 1);</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GESTION DE TECNOLOGIA', 'GESTION DE TECNOLOGIA', RAND(), 20.1, 120.5, 'OLVIDO DE CONTRASEÑAS Y PROBLEMAS DE INGRESO A LOS SISTEMAS AQUÍ TE SOLUCIONARAN', 1);</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" t="s">
-        <v>72</v>
+        <v>23</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'DECANATURA INGENIERIA', 'DECANATURA INGENIERIA', 'www.autonoma.edu.co/gestion_de_tecnologia', '20,120', 'OLVIDO DE CONTRASEÑAS Y PROBLEMAS DE INGRESO A LOS SISTEMAS AQUÍ TE SOLUCIONARAN', 1);</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G14" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DECANATURA INGENIERIA', 'DECANATURA INGENIERIA', RAND(), 20.1, 120.5, 'LOS PROCESOS ACADEMICOS DESDE ALLÍ SE GOBERNARAN', 1);</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
+        <v>36</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'SALA DE PROFESORES DE INGENIERIA', 'SALA DE PROFESORES DE INGENIERIA', 'www.autonoma.edu.co/decanatura_ingenieria', '20,120', 'LOS PROCESOS ACADEMICOS DESDE ALLÍ SE GOBERNARAN', 1);</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SALA DE PROFESORES DE INGENIERIA', 'SALA DE PROFESORES DE INGENIERIA', RAND(), 20.1, 120.5, 'ASISTENCIA Y CONSULTARIA DE QUIENES TE ENSEÑAN EN ESTE LUGAR TENDRAS', 1);</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" t="s">
-        <v>74</v>
+        <v>31</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>117</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'CENTRO DE INFORMATICA', 'CENTRO DE INFORMATICA', 'www.autonoma.edu.co/sala_de_profesores_de_ingenieria', '20,120', 'ASISTENCIA Y CONSULTARIA DE QUIENES TE ENSEÑAN EN ESTE LUGAR TENDRAS', 1);</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CENTRO DE INFORMATICA', 'CENTRO DE INFORMATICA', RAND(), 20.1, 120.5, 'LAS HERRAMIENTAS COMPUTACIONES EN ESTE PISO ENTERO ENCONTRARAS', 1);</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G17" t="s">
         <v>75</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'VICERRECTORIA ACADEMICA', 'VICERRECTORIA ACADEMICA', 'www.autonoma.edu.co/centro_de_informatica', '20,120', 'LAS HERRAMIENTAS COMPUTACIONES EN ESTE PISO ENTERO ENCONTRARAS', 1);</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'VICERRECTORIA ACADEMICA', 'VICERRECTORIA ACADEMICA', RAND(), 20.1, 120.5, 'CUANDO PROBLEMAS ACADÉMICOS ENCUENTRES, ESTE ES EL MÁXIMO ESTAMENTO A CONSULTAR', 1);</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F18" t="s">
-        <v>102</v>
-      </c>
-      <c r="G18">
-        <v>1</v>
-      </c>
-      <c r="H18" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'RECTORIA', 'RECTORIA', 'www.autonoma.edu.co/vicerrectoria_academica', '20,120', 'CUANDO PROBLEMAS ACADÉMICOS ENCUENTRES, ESTE ES EL MÁXIMO ESTAMENTO A CONSULTAR', 1);</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RECTORIA', 'RECTORIA', RAND(), 20.1, 120.5, 'DESDE ALLÍ SE DIRIGE LA UAM', 1);</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19">
-        <v>1</v>
-      </c>
-      <c r="H19" t="str">
-        <f t="shared" si="0"/>
-        <v>INSERT  INTO nodo (nombre, descripcion,codigo, ubicacion, pista, carreraId) VALUES ( 'VICERRECTORIA ADMINISTRATIVA', 'VICERRECTORIA ADMINISTRATIVA', 'www.autonoma.edu.co/rectoria', '20,120', 'DESDE ALLÍ SE DIRIGE LA UAM', 1);</v>
+        <v>125</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G19" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 20.1, 120.5, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 20.1, 120.5, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 2);</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G21" t="s">
+        <v>13</v>
+      </c>
+      <c r="H21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 20.1, 120.5, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 2);</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D18" r:id="rId2"/>
-    <hyperlink ref="D19" r:id="rId3"/>
+    <hyperlink ref="D2" r:id="rId1" display="www.autonoma.edu.co/biblioteca"/>
+    <hyperlink ref="D3:D18" r:id="rId2" display="www.autonoma.edu.co/biblioteca"/>
+    <hyperlink ref="D19" r:id="rId3" display="www.autonoma.edu.co/biblioteca"/>
+    <hyperlink ref="D20:D21" r:id="rId4" display="www.autonoma.edu.co/biblioteca"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1521,13 +1605,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>123</v>
       </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1536,17 +1620,17 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="F2" t="str">
-        <f>CONCATENATE("INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES (", " '",B2,"', '",C2, "', ",D2,");")</f>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'WBEIMAR CANO RESTREPO', 1);</v>
+        <f>CONCATENATE("INSERT  INTO question (question, answer, node_id) VALUES (", " '",B2,"', '",C2, "', ",D2,");")</f>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'WBEIMAR CANO RESTREPO', 1);</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1554,17 +1638,17 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F32" si="0">CONCATENATE("INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES (", " '",B3,"', '",C3, "', ",D3,");")</f>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA ZONA EN QUE ENCONTRARÁS REVISTAS ESPECIALIZADAS?', 'HEMEROTECA', 1);</v>
+        <f t="shared" ref="F3:F40" si="0">CONCATENATE("INSERT  INTO question (question, answer, node_id) VALUES (", " '",B3,"', '",C3, "', ",D3,");")</f>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA ZONA EN QUE ENCONTRARÁS REVISTAS ESPECIALIZADAS?', 'HEMEROTECA', 1);</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1572,17 +1656,17 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DE CONSULTA ELECTRÓNICA?', 'TELEMATICA', 1);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DE CONSULTA ELECTRÓNICA?', 'TELEMATICA', 1);</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1590,17 +1674,17 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DONDE VIDEOS Y PELÍCULAS PUEDES ENCONTRAR?', 'VIDEOTECA', 1);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DONDE VIDEOS Y PELÍCULAS PUEDES ENCONTRAR?', 'VIDEOTECA', 1);</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,17 +1692,17 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿QUÉ BASE DE DATOS PUEDES CONSULTAR SI DIRECTAMENTE ARTÍCULOS CIENTÍFICOS QUIERES ENCONTRAR?', 'SCIENCE DIRECT', 1);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿QUÉ BASE DE DATOS PUEDES CONSULTAR SI DIRECTAMENTE ARTÍCULOS CIENTÍFICOS QUIERES ENCONTRAR?', 'SCIENCE DIRECT', 1);</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1626,17 +1710,17 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="C7" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="D7">
         <v>2</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA PERSONA QUE SIEMPRE ENCUENTRAS EN ESTE LUGAR?', 'JHON JAMES LOPEZ', 2);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA PERSONA QUE SIEMPRE ENCUENTRAS EN ESTE LUGAR?', 'JHON JAMES LOPEZ', 2);</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1644,17 +1728,17 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>82</v>
+        <v>56</v>
       </c>
       <c r="D8">
         <v>2</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿ADEMÁS DE LA MATRÍCULA ESTOS ELEMENTOS DE ESTUDIO ACÁ PUEDES PAGAR PARA LUEGO EN EL ALMACÉN RECLAMAR?', 'LIBROS', 2);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿ADEMÁS DE LA MATRÍCULA ESTOS ELEMENTOS DE ESTUDIO ACÁ PUEDES PAGAR PARA LUEGO EN EL ALMACÉN RECLAMAR?', 'LIBROS', 2);</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,17 +1746,17 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>84</v>
+        <v>58</v>
       </c>
       <c r="D9">
         <v>3</v>
       </c>
       <c r="F9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'YHON HENRY BARRETO MIRANDA', 3);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'YHON HENRY BARRETO MIRANDA', 3);</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1680,17 +1764,17 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <v>3</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿QUÉ DOCUMENTO TE ENTREGARÁN EN ÉSTE LUGAR QUE TE SERVIRÁ PARA IDENTIFICARTE E INGRESAR A LA UAM?', 'CARNET ESTUDIANTIL', 3);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿QUÉ DOCUMENTO TE ENTREGARÁN EN ÉSTE LUGAR QUE TE SERVIRÁ PARA IDENTIFICARTE E INGRESAR A LA UAM?', 'CARNET ESTUDIANTIL', 3);</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1698,17 +1782,17 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="D11">
         <v>4</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'SONIA PATRICIA VILLAMIL RODRIGUEZ', 4);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'SONIA PATRICIA VILLAMIL RODRIGUEZ', 4);</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1716,17 +1800,17 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>85</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿INDICA CUAL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?', 'SERVICIOALCLIENTE@AUTONOMA.EDU.CO', 4);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿INDICA CUAL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?', 'SERVICIOALCLIENTE@AUTONOMA.EDU.CO', 4);</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1734,17 +1818,17 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>87</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="D13">
         <v>5</v>
       </c>
       <c r="F13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL PROGRAMA DE MOVILIDAD ACADEMICA ENTRE COLOMBIA Y ARGENTINA?', 'MACA', 5);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL PROGRAMA DE MOVILIDAD ACADEMICA ENTRE COLOMBIA Y ARGENTINA?', 'MACA', 5);</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1752,17 +1836,17 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>89</v>
+        <v>63</v>
       </c>
       <c r="D14">
         <v>5</v>
       </c>
       <c r="F14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'VIVIANA FERNANDA NIETO PADILLA', 5);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'VIVIANA FERNANDA NIETO PADILLA', 5);</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1770,17 +1854,17 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D15">
         <v>6</v>
       </c>
       <c r="F15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'CARMENZA GONZALEZ BURITICA', 6);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'CARMENZA GONZALEZ BURITICA', 6);</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1788,17 +1872,17 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="D16">
         <v>6</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( 'DE ESTA INSTITUCIÓN GUBERNAMENTAL UN DELEGADO EN ESTA OFICINA ENCONTRARÁS, ¿CUAL ES SU NOMBRE?', 'ICETEX', 6);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( 'DE ESTA INSTITUCIÓN GUBERNAMENTAL UN DELEGADO EN ESTA OFICINA ENCONTRARÁS, ¿CUAL ES SU NOMBRE?', 'ICETEX', 6);</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1806,17 +1890,17 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D17">
         <v>7</v>
       </c>
       <c r="F17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿NOMBRA AL VICERRECTOR DE DESARROLLO HUMANO?', 'ALBERTO CARDONA AGUIRRE', 7);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿NOMBRA AL VICERRECTOR DE DESARROLLO HUMANO?', 'ALBERTO CARDONA AGUIRRE', 7);</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1824,17 +1908,17 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="D18">
         <v>8</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿ELLA ES LA ENCARGADA DE ASIGNARTE CITAS Y RECIBIRTE EN ESTE LUGAR?', 'IRENE MARULANDA SALGADO', 8);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿ELLA ES LA ENCARGADA DE ASIGNARTE CITAS Y RECIBIRTE EN ESTE LUGAR?', 'IRENE MARULANDA SALGADO', 8);</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1842,17 +1926,17 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="D19">
         <v>9</v>
       </c>
       <c r="F19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿ES UNO DE LOS ENCARGADOS Y SU PRIMER NOMBRE INICIA CON L Y EL SEGUNDO CON C?', 'LUIS CARLOS RIOS DIAZ', 9);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿ES UNO DE LOS ENCARGADOS Y SU PRIMER NOMBRE INICIA CON L Y EL SEGUNDO CON C?', 'LUIS CARLOS RIOS DIAZ', 9);</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,17 +1944,17 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="D20">
         <v>10</v>
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'HISNEL FRANCO MARQUEZ', 10);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'HISNEL FRANCO MARQUEZ', 10);</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1878,17 +1962,17 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>114</v>
+        <v>83</v>
       </c>
       <c r="D21">
         <v>11</v>
       </c>
       <c r="F21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿DI EL NOMBRE CON EL QUE SE CONOCE EL EDIFICIO EN QUE SE ENCUENTRA EL GIMNASIO?', 'SACATIN', 11);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿DI EL NOMBRE CON EL QUE SE CONOCE EL EDIFICIO EN QUE SE ENCUENTRA EL GIMNASIO?', 'SACATIN', 11);</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,17 +1980,17 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>142</v>
+        <v>104</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>143</v>
+        <v>105</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL CORRE DE ATENCIÓN GENERAL DE ESTE LUGAR?', 'GESTEC@AUTONOMA.EDU.CO', 12);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL CORRE DE ATENCIÓN GENERAL DE ESTE LUGAR?', 'GESTEC@AUTONOMA.EDU.CO', 12);</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1914,17 +1998,17 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="D23">
         <v>12</v>
       </c>
       <c r="F23" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA COMUNITY MANAGER UAM?', 'MARGARITA BENAVIDES', 12);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA COMUNITY MANAGER UAM?', 'MARGARITA BENAVIDES', 12);</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1932,17 +2016,17 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
+        <v>84</v>
       </c>
       <c r="C24" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="D24">
         <v>13</v>
       </c>
       <c r="F24" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUÁL ES EL NOMBRE DE LA DECANO DE INGENIERIA?', 'ALBA PATRICIA ARIAS OSORIO', 13);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA DECANO DE INGENIERIA?', 'ALBA PATRICIA ARIAS OSORIO', 13);</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1950,17 +2034,17 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="D25">
         <v>13</v>
       </c>
       <c r="F25" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUAL ES EL NOMBRE DE LA AUXILIAR ADMINISTRATIVA DE INGENIERÍA EN EL DÍA?', 'BEATRIZ ALVARAN DAVILA', 13);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUAL ES EL NOMBRE DE LA AUXILIAR ADMINISTRATIVA DE INGENIERÍA EN EL DÍA?', 'BEATRIZ ALVARAN DAVILA', 13);</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1968,17 +2052,17 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="D26">
         <v>13</v>
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUAL ES EL NOMBRE DE LA AUXILIAR ADMINISTRATIVA DE INGENIERÍA EN LA NOCHE?', 'INES ARGELIA LOAIZA GARZON', 13);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUAL ES EL NOMBRE DE LA AUXILIAR ADMINISTRATIVA DE INGENIERÍA EN LA NOCHE?', 'INES ARGELIA LOAIZA GARZON', 13);</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1986,17 +2070,17 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
       <c r="C27" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
       <c r="D27">
         <v>14</v>
       </c>
       <c r="F27" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿CUAL ES EL NOMBRE DE LA COORDINADORA DEL PROGRAMA DE INGENIERIA?', 'LINA MARIA LOPEZ URIBE', 14);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUAL ES EL NOMBRE DE LA COORDINADORA DEL PROGRAMA DE INGENIERIA?', 'LINA MARIA LOPEZ URIBE', 14);</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -2004,17 +2088,17 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="C28" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
       <c r="D28">
         <v>14</v>
       </c>
       <c r="F28" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿NOMBRA AL PROFESOR CUYO CORREO ES JIMEZAM?', 'JORGE IVAN MEZA MARTINEZ', 14);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿NOMBRA AL PROFESOR CUYO CORREO ES JIMEZAM?', 'JORGE IVAN MEZA MARTINEZ', 14);</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -2022,17 +2106,17 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
       <c r="D29">
         <v>15</v>
       </c>
       <c r="F29" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿INDICA EL NOMBRE DE LA ENCARGADA DEL CENTRO DE INFORMATICA?', 'MARTHA LILIA MORALES GONZALEZ', 15);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿INDICA EL NOMBRE DE LA ENCARGADA DEL CENTRO DE INFORMATICA?', 'MARTHA LILIA MORALES GONZALEZ', 15);</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -2040,17 +2124,17 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D30">
         <v>16</v>
       </c>
       <c r="F30" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿NOMBRA AL VICERRECTOR ACADEMICO DE LA UAM?', 'IVAN ESCOBAR ESCOBAR', 16);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿NOMBRA AL VICERRECTOR ACADEMICO DE LA UAM?', 'IVAN ESCOBAR ESCOBAR', 16);</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -2058,35 +2142,179 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="C31" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="D31">
         <v>17</v>
       </c>
       <c r="F31" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿NOMBRA AL RECTOR DE LA INSTITUCION?', 'GABRIEL CADENA GOMEZ', 17);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿NOMBRA AL RECTOR DE LA INSTITUCION?', 'GABRIEL CADENA GOMEZ', 17);</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>14</v>
       </c>
       <c r="C32" t="s">
-        <v>107</v>
+        <v>15</v>
       </c>
       <c r="D32">
         <v>18</v>
       </c>
       <c r="F32" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO pregunta (enunciado, respuesta, nodoId) VALUES ( '¿NOMBRA AL VICERRECTOR ADMINISTRATIVO DE LA UAM?', 'CARLOS EDUARDO JARAMILLO SANINT', 18);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'WBEIMAR CANO RESTREPO', 18);</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C33" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>18</v>
+      </c>
+      <c r="F33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA ZONA EN QUE ENCONTRARÁS REVISTAS ESPECIALIZADAS?', 'HEMEROTECA', 18);</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34">
+        <v>18</v>
+      </c>
+      <c r="F34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DE CONSULTA ELECTRÓNICA?', 'TELEMATICA', 18);</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <v>18</v>
+      </c>
+      <c r="F35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA SALA DONDE VIDEOS Y PELÍCULAS PUEDES ENCONTRAR?', 'VIDEOTECA', 18);</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>18</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿QUÉ BASE DE DATOS PUEDES CONSULTAR SI DIRECTAMENTE ARTÍCULOS CIENTÍFICOS QUIERES ENCONTRAR?', 'SCIENCE DIRECT', 18);</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>53</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37">
+        <v>19</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DE LA PERSONA QUE SIEMPRE ENCUENTRAS EN ESTE LUGAR?', 'JHON JAMES LOPEZ', 19);</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D38">
+        <v>19</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿ADEMÁS DE LA MATRÍCULA ESTOS ELEMENTOS DE ESTUDIO ACÁ PUEDES PAGAR PARA LUEGO EN EL ALMACÉN RECLAMAR?', 'LIBROS', 19);</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39">
+        <v>19</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL NOMBRE DEL COORDINADOR DE ÉSTE LUGAR?', 'YHON HENRY BARRETO MIRANDA', 19);</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40">
+        <v>20</v>
+      </c>
+      <c r="F40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿QUÉ DOCUMENTO TE ENTREGARÁN EN ÉSTE LUGAR QUE TE SERVIRÁ PARA IDENTIFICARTE E INGRESAR A LA UAM?', 'CARNET ESTUDIANTIL', 20);</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tabla estado competencia terminada
</commit_message>
<xml_diff>
--- a/CarreraObsGenerador.xlsx
+++ b/CarreraObsGenerador.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Carrera" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="158">
   <si>
     <t>id</t>
   </si>
@@ -404,10 +404,103 @@
     <t>node_id</t>
   </si>
   <si>
-    <t>20.1</t>
-  </si>
-  <si>
-    <t>120.5</t>
+    <t>5.0672036513457535</t>
+  </si>
+  <si>
+    <t>-75.5031082034111</t>
+  </si>
+  <si>
+    <t>5.067820819841856</t>
+  </si>
+  <si>
+    <t>-75.50278767943382</t>
+  </si>
+  <si>
+    <t>5.067927688785628</t>
+  </si>
+  <si>
+    <t>-75.50267234444618</t>
+  </si>
+  <si>
+    <t>5.067828835013248</t>
+  </si>
+  <si>
+    <t>-75.50270587205887</t>
+  </si>
+  <si>
+    <t>5.067871582592347</t>
+  </si>
+  <si>
+    <t>-75.50261199474335</t>
+  </si>
+  <si>
+    <t>-75.50262004137039</t>
+  </si>
+  <si>
+    <t>5.068297722366866</t>
+  </si>
+  <si>
+    <t>-75.50283528864384</t>
+  </si>
+  <si>
+    <t>5.0685234828231644</t>
+  </si>
+  <si>
+    <t>-75.50286144018173</t>
+  </si>
+  <si>
+    <t>5.0682402803446776</t>
+  </si>
+  <si>
+    <t>-75.50261467695236</t>
+  </si>
+  <si>
+    <t>5.068512795939442</t>
+  </si>
+  <si>
+    <t>-75.50254493951797</t>
+  </si>
+  <si>
+    <t>5.068566230356298</t>
+  </si>
+  <si>
+    <t>-75.50263077020645</t>
+  </si>
+  <si>
+    <t>5.068304401671438</t>
+  </si>
+  <si>
+    <t>-75.50262540578842</t>
+  </si>
+  <si>
+    <t>5.068534169706709</t>
+  </si>
+  <si>
+    <t>-75.50278097391129</t>
+  </si>
+  <si>
+    <t>5.068763937660251</t>
+  </si>
+  <si>
+    <t>-75.50281316041946</t>
+  </si>
+  <si>
+    <t>5.067786087431325</t>
+  </si>
+  <si>
+    <t>-75.50275951623917</t>
+  </si>
+  <si>
+    <t>5.066808235722423</t>
+  </si>
+  <si>
+    <t>-75.50553292036057</t>
+  </si>
+  <si>
+    <t>5.06676548807297</t>
+  </si>
+  <si>
+    <t>-75.5052325129509</t>
   </si>
 </sst>
 </file>
@@ -930,21 +1023,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I21" sqref="I2:I21"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="111.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="255.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1001,7 +1091,7 @@
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES (", " '",B2,"', '",C2, "', ",D2,", ",E2,", ",F2, ", '",G2,"', ",H2,");")</f>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 20.1, 120.5, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 5.0672036513457535, -75.5031082034111, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1018,10 +1108,10 @@
         <v>117</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
         <v>37</v>
@@ -1031,7 +1121,7 @@
       </c>
       <c r="I3" t="str">
         <f t="shared" ref="I3:I21" si="0">CONCATENATE("INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES (", " '",B3,"', '",C3, "', ",D3,", ",E3,", ",F3, ", '",G3,"', ",H3,");")</f>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 20.1, 120.5, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 5.067820819841856, -75.50278767943382, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 1);</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1048,10 +1138,10 @@
         <v>117</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -1061,7 +1151,7 @@
       </c>
       <c r="I4" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 20.1, 120.5, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 5.067927688785628, -75.50267234444618, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 1);</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1078,10 +1168,10 @@
         <v>117</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -1091,7 +1181,7 @@
       </c>
       <c r="I5" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'MERCADEO', 'MERCADEO', RAND(), 20.1, 120.5, 'SUS ENCARGADOS LA OFERTA ACADEMICA Y AYUDA ADMINISTRATIVA TE OFRECERAN', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'MERCADEO', 'MERCADEO', RAND(), 5.067828835013248, -75.50270587205887, 'SUS ENCARGADOS LA OFERTA ACADEMICA Y AYUDA ADMINISTRATIVA TE OFRECERAN', 1);</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1108,10 +1198,10 @@
         <v>117</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="G6" t="s">
         <v>39</v>
@@ -1121,7 +1211,7 @@
       </c>
       <c r="I6" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RELACIONES INTERNACIONALES', 'RELACIONES INTERNACIONALES', RAND(), 20.1, 120.5, 'SI UN INTERCAMBIO QUIERES HACER A ESTE LUGAR DEBES LLEGAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RELACIONES INTERNACIONALES', 'RELACIONES INTERNACIONALES', RAND(), 5.067871582592347, -75.50261199474335, 'SI UN INTERCAMBIO QUIERES HACER A ESTE LUGAR DEBES LLEGAR', 1);</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1138,10 +1228,10 @@
         <v>117</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -1151,7 +1241,7 @@
       </c>
       <c r="I7" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CARTERA', 'CARTERA', RAND(), 20.1, 120.5, 'PLAZOS DE FINANCIAMIENTO Y OPCIONES A PROBLEMAS ECONOMICAS ACA TE DARAN', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CARTERA', 'CARTERA', RAND(), 5.067828835013248, -75.50262004137039, 'PLAZOS DE FINANCIAMIENTO Y OPCIONES A PROBLEMAS ECONOMICAS ACA TE DARAN', 1);</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1168,10 +1258,10 @@
         <v>117</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="G8" t="s">
         <v>41</v>
@@ -1181,7 +1271,7 @@
       </c>
       <c r="I8" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DESARROLLO HUMANO', 'DESARROLLO HUMANO', RAND(), 20.1, 120.5, 'SUS ENCARGADOS VELAN POR TU BIENESTAR MENTAL Y PSICOLOGICO, ADEMAS DE AYUDA CON DIFICULTADES ACADEMICAS', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DESARROLLO HUMANO', 'DESARROLLO HUMANO', RAND(), 5.068297722366866, -75.50283528864384, 'SUS ENCARGADOS VELAN POR TU BIENESTAR MENTAL Y PSICOLOGICO, ADEMAS DE AYUDA CON DIFICULTADES ACADEMICAS', 1);</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1198,10 +1288,10 @@
         <v>117</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="G9" t="s">
         <v>42</v>
@@ -1211,7 +1301,7 @@
       </c>
       <c r="I9" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SERVICIOS MEDICOS', 'SERVICIOS MEDICOS', RAND(), 20.1, 120.5, 'EN ESTE SITIO ENCONTRARAS UN MEDICO QUE TE PUEDE INDICAR QUE TRATAMIENTO TOMAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SERVICIOS MEDICOS', 'SERVICIOS MEDICOS', RAND(), 5.0685234828231644, -75.50286144018173, 'EN ESTE SITIO ENCONTRARAS UN MEDICO QUE TE PUEDE INDICAR QUE TRATAMIENTO TOMAR', 1);</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1228,10 +1318,10 @@
         <v>117</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
@@ -1241,7 +1331,7 @@
       </c>
       <c r="I10" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'ATENCION PREHOSPITALARIA', 'ATENCION PREHOSPITALARIA', RAND(), 20.1, 120.5, 'SI TE SIENTES FISICAMENTE MAL EN ESTE LUGAR UNA PERSONA PROFESIONAL TE ATENDERA', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'ATENCION PREHOSPITALARIA', 'ATENCION PREHOSPITALARIA', RAND(), 5.0682402803446776, -75.50261467695236, 'SI TE SIENTES FISICAMENTE MAL EN ESTE LUGAR UNA PERSONA PROFESIONAL TE ATENDERA', 1);</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1258,10 +1348,10 @@
         <v>117</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
@@ -1271,7 +1361,7 @@
       </c>
       <c r="I11" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'LABORATORIO ELECTRONICA', 'LABORATORIO ELECTRONICA', RAND(), 20.1, 120.5, 'LOS MONTAJES ELECTRONICOS Y EXPERIMENTOS FISICOS EN ESTE LUGAR DESARROLLARAS', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'LABORATORIO ELECTRONICA', 'LABORATORIO ELECTRONICA', RAND(), 5.068512795939442, -75.50254493951797, 'LOS MONTAJES ELECTRONICOS Y EXPERIMENTOS FISICOS EN ESTE LUGAR DESARROLLARAS', 1);</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1288,10 +1378,10 @@
         <v>117</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
       <c r="G12" t="s">
         <v>45</v>
@@ -1301,7 +1391,7 @@
       </c>
       <c r="I12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GIMNASIO', 'GIMNASIO', RAND(), 20.1, 120.5, 'ALLI EJERCICIO, JUGAR Y LIBERAR TENSION PUEDES REALIZAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GIMNASIO', 'GIMNASIO', RAND(), 5.068566230356298, -75.50263077020645, 'ALLI EJERCICIO, JUGAR Y LIBERAR TENSION PUEDES REALIZAR', 1);</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1318,10 +1408,10 @@
         <v>117</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="G13" t="s">
         <v>46</v>
@@ -1331,7 +1421,7 @@
       </c>
       <c r="I13" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GESTION DE TECNOLOGIA', 'GESTION DE TECNOLOGIA', RAND(), 20.1, 120.5, 'OLVIDO DE CONTRASEÑAS Y PROBLEMAS DE INGRESO A LOS SISTEMAS AQUÍ TE SOLUCIONARAN', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'GESTION DE TECNOLOGIA', 'GESTION DE TECNOLOGIA', RAND(), 5.068304401671438, -75.50262540578842, 'OLVIDO DE CONTRASEÑAS Y PROBLEMAS DE INGRESO A LOS SISTEMAS AQUÍ TE SOLUCIONARAN', 1);</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1348,10 +1438,10 @@
         <v>117</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="G14" t="s">
         <v>47</v>
@@ -1361,7 +1451,7 @@
       </c>
       <c r="I14" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DECANATURA INGENIERIA', 'DECANATURA INGENIERIA', RAND(), 20.1, 120.5, 'LOS PROCESOS ACADEMICOS DESDE ALLÍ SE GOBERNARAN', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'DECANATURA INGENIERIA', 'DECANATURA INGENIERIA', RAND(), 5.068534169706709, -75.50278097391129, 'LOS PROCESOS ACADEMICOS DESDE ALLÍ SE GOBERNARAN', 1);</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1378,10 +1468,10 @@
         <v>117</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>125</v>
+        <v>150</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>126</v>
+        <v>151</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
@@ -1391,7 +1481,7 @@
       </c>
       <c r="I15" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SALA DE PROFESORES DE INGENIERIA', 'SALA DE PROFESORES DE INGENIERIA', RAND(), 20.1, 120.5, 'ASISTENCIA Y CONSULTARIA DE QUIENES TE ENSEÑAN EN ESTE LUGAR TENDRAS', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'SALA DE PROFESORES DE INGENIERIA', 'SALA DE PROFESORES DE INGENIERIA', RAND(), 5.068763937660251, -75.50281316041946, 'ASISTENCIA Y CONSULTARIA DE QUIENES TE ENSEÑAN EN ESTE LUGAR TENDRAS', 1);</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1408,10 +1498,10 @@
         <v>117</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="G16" t="s">
         <v>49</v>
@@ -1421,7 +1511,7 @@
       </c>
       <c r="I16" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CENTRO DE INFORMATICA', 'CENTRO DE INFORMATICA', RAND(), 20.1, 120.5, 'LAS HERRAMIENTAS COMPUTACIONES EN ESTE PISO ENTERO ENCONTRARAS', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CENTRO DE INFORMATICA', 'CENTRO DE INFORMATICA', RAND(), 5.067786087431325, -75.50275951623917, 'LAS HERRAMIENTAS COMPUTACIONES EN ESTE PISO ENTERO ENCONTRARAS', 1);</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1438,10 +1528,10 @@
         <v>117</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G17" t="s">
         <v>75</v>
@@ -1451,7 +1541,7 @@
       </c>
       <c r="I17" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'VICERRECTORIA ACADEMICA', 'VICERRECTORIA ACADEMICA', RAND(), 20.1, 120.5, 'CUANDO PROBLEMAS ACADÉMICOS ENCUENTRES, ESTE ES EL MÁXIMO ESTAMENTO A CONSULTAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'VICERRECTORIA ACADEMICA', 'VICERRECTORIA ACADEMICA', RAND(), 5.066808235722423, -75.50553292036057, 'CUANDO PROBLEMAS ACADÉMICOS ENCUENTRES, ESTE ES EL MÁXIMO ESTAMENTO A CONSULTAR', 1);</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1468,10 +1558,10 @@
         <v>117</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
       <c r="G18" t="s">
         <v>76</v>
@@ -1481,7 +1571,7 @@
       </c>
       <c r="I18" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RECTORIA', 'RECTORIA', RAND(), 20.1, 120.5, 'DESDE ALLÍ SE DIRIGE LA UAM', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'RECTORIA', 'RECTORIA', RAND(), 5.06676548807297, -75.5052325129509, 'DESDE ALLÍ SE DIRIGE LA UAM', 1);</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1511,7 +1601,7 @@
       </c>
       <c r="I19" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 20.1, 120.5, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'BIBLIOTECA', 'BIBLIOTECA', RAND(), 5.0672036513457535, -75.5031082034111, 'SILENCIO, ESPACIO Y CONOCIMIENTO ENCONTRARAS EN ESTE LUGAR', 1);</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1528,10 +1618,10 @@
         <v>117</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -1541,7 +1631,7 @@
       </c>
       <c r="I20" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 20.1, 120.5, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 2);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'CAJA', 'CAJA', RAND(), 5.067820819841856, -75.50278767943382, 'AQUÍ TU SEMESTRE Y LIBROS HAS DE PAGAR', 2);</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1558,10 +1648,10 @@
         <v>117</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -1571,7 +1661,7 @@
       </c>
       <c r="I21" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 20.1, 120.5, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 2);</v>
+        <v>INSERT  INTO node (name, description,code, latitude, longitude, hint,  circuit_Id) VALUES ( 'REGISTRO ACADEMICO', 'REGISTRO ACADEMICO', RAND(), 5.067927688785628, -75.50267234444618, 'EN ESTE LUGAR EL PROCESO DE INSCRIPCION ACENTARAS', 2);</v>
       </c>
     </row>
   </sheetData>
@@ -1590,7 +1680,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Estilos y apariencia terminados
</commit_message>
<xml_diff>
--- a/CarreraObsGenerador.xlsx
+++ b/CarreraObsGenerador.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Carrera" sheetId="1" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>YHON HENRY BARRETO MIRANDA</t>
   </si>
   <si>
-    <t>¿INDICA CUAL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?</t>
-  </si>
-  <si>
     <t>SERVICIOALCLIENTE@AUTONOMA.EDU.CO</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
     <t>14/04/1978</t>
   </si>
   <si>
-    <t>¿CUÁL ES EL CORRE DE ATENCIÓN GENERAL DE ESTE LUGAR?</t>
-  </si>
-  <si>
     <t>GESTEC@AUTONOMA.EDU.CO</t>
   </si>
   <si>
@@ -501,6 +495,12 @@
   </si>
   <si>
     <t>-75.5052325129509</t>
+  </si>
+  <si>
+    <t>¿INDICA CUÁL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?</t>
+  </si>
+  <si>
+    <t>¿CUÁL ES EL CORREO DE ATENCIÓN GENERAL DE ESTE LUGAR?</t>
   </si>
 </sst>
 </file>
@@ -852,13 +852,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
-        <v>108</v>
-      </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -872,7 +872,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E2" t="str">
         <f>CONCATENATE("INSERT  INTO circuit (name, status, description) VALUES ('",B2,"', ",C2,",'",D2, "');")</f>
@@ -884,13 +884,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E3" t="str">
         <f>CONCATENATE("INSERT  INTO circuit (name, status, description) VALUES ('",B3,"', ",C3,",'",D3, "');")</f>
@@ -928,25 +928,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>111</v>
-      </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -960,7 +960,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>3</v>
@@ -969,10 +969,10 @@
         <v>6</v>
       </c>
       <c r="G2" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" t="s">
         <v>99</v>
-      </c>
-      <c r="H2" t="s">
-        <v>100</v>
       </c>
       <c r="I2" t="str">
         <f>CONCATENATE("INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES (","'",B2, "', '",C2,"', '",D2, "', '",E2,"', '",F2, "', '",G2,"','",H2,"');")</f>
@@ -990,7 +990,7 @@
         <v>9</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>7</v>
@@ -999,10 +999,10 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I3" t="str">
         <f>CONCATENATE("INSERT  INTO user (name, lastname. birthDate, email, color, gender, type) VALUES (","'",B3, "', '",C3,"', '",D3, "', '",E3,"', '",F3, "', '",G3,"','",H3,"');")</f>
@@ -1023,7 +1023,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1042,25 +1042,25 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>117</v>
+      </c>
+      <c r="G1" t="s">
         <v>118</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>119</v>
-      </c>
-      <c r="G1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H1" t="s">
-        <v>121</v>
       </c>
       <c r="I1" s="1"/>
     </row>
@@ -1075,13 +1075,13 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>12</v>
@@ -1105,13 +1105,13 @@
         <v>24</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G3" t="s">
         <v>37</v>
@@ -1135,13 +1135,13 @@
         <v>33</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G4" t="s">
         <v>13</v>
@@ -1165,13 +1165,13 @@
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G5" t="s">
         <v>38</v>
@@ -1195,13 +1195,13 @@
         <v>34</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G6" t="s">
         <v>39</v>
@@ -1225,13 +1225,13 @@
         <v>26</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G7" t="s">
         <v>40</v>
@@ -1255,13 +1255,13 @@
         <v>27</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G8" t="s">
         <v>41</v>
@@ -1285,13 +1285,13 @@
         <v>28</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G9" t="s">
         <v>42</v>
@@ -1315,13 +1315,13 @@
         <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G10" t="s">
         <v>44</v>
@@ -1345,13 +1345,13 @@
         <v>30</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G11" t="s">
         <v>43</v>
@@ -1375,13 +1375,13 @@
         <v>29</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G12" t="s">
         <v>45</v>
@@ -1405,13 +1405,13 @@
         <v>22</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G13" t="s">
         <v>46</v>
@@ -1435,13 +1435,13 @@
         <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G14" t="s">
         <v>47</v>
@@ -1465,13 +1465,13 @@
         <v>36</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G15" t="s">
         <v>48</v>
@@ -1495,13 +1495,13 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G16" t="s">
         <v>49</v>
@@ -1519,22 +1519,22 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -1549,22 +1549,22 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -1585,13 +1585,13 @@
         <v>11</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -1615,13 +1615,13 @@
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="G20" t="s">
         <v>37</v>
@@ -1645,13 +1645,13 @@
         <v>33</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
         <v>13</v>
@@ -1680,8 +1680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1695,13 +1695,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
         <v>122</v>
-      </c>
-      <c r="C1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D1" t="s">
-        <v>124</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -1890,17 +1890,17 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="D12">
         <v>4</v>
       </c>
       <c r="F12" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿INDICA CUAL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?', 'SERVICIOALCLIENTE@AUTONOMA.EDU.CO', 4);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿INDICA CUÁL ES EL CORREO GENERAL DE MERCADEO Y SERVICIO AL CLIENTE?', 'SERVICIOALCLIENTE@AUTONOMA.EDU.CO', 4);</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1908,10 +1908,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
         <v>61</v>
-      </c>
-      <c r="C13" t="s">
-        <v>62</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1929,7 +1929,7 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -1947,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D15">
         <v>6</v>
@@ -1962,10 +1962,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" t="s">
         <v>65</v>
-      </c>
-      <c r="C16" t="s">
-        <v>66</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -1980,10 +1980,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" t="s">
         <v>67</v>
-      </c>
-      <c r="C17" t="s">
-        <v>68</v>
       </c>
       <c r="D17">
         <v>7</v>
@@ -1998,10 +1998,10 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" t="s">
         <v>77</v>
-      </c>
-      <c r="C18" t="s">
-        <v>78</v>
       </c>
       <c r="D18">
         <v>8</v>
@@ -2016,10 +2016,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D19">
         <v>9</v>
@@ -2037,7 +2037,7 @@
         <v>14</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -2052,10 +2052,10 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" t="s">
         <v>82</v>
-      </c>
-      <c r="C21" t="s">
-        <v>83</v>
       </c>
       <c r="D21">
         <v>11</v>
@@ -2070,17 +2070,17 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>104</v>
+        <v>157</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D22">
         <v>12</v>
       </c>
       <c r="F22" t="str">
         <f t="shared" si="0"/>
-        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL CORRE DE ATENCIÓN GENERAL DE ESTE LUGAR?', 'GESTEC@AUTONOMA.EDU.CO', 12);</v>
+        <v>INSERT  INTO question (question, answer, node_id) VALUES ( '¿CUÁL ES EL CORREO DE ATENCIÓN GENERAL DE ESTE LUGAR?', 'GESTEC@AUTONOMA.EDU.CO', 12);</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -2088,10 +2088,10 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>85</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
       </c>
       <c r="D23">
         <v>12</v>
@@ -2106,10 +2106,10 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" t="s">
-        <v>85</v>
       </c>
       <c r="D24">
         <v>13</v>
@@ -2124,10 +2124,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" t="s">
         <v>88</v>
-      </c>
-      <c r="C25" t="s">
-        <v>89</v>
       </c>
       <c r="D25">
         <v>13</v>
@@ -2142,10 +2142,10 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
+        <v>89</v>
+      </c>
+      <c r="C26" t="s">
         <v>90</v>
-      </c>
-      <c r="C26" t="s">
-        <v>91</v>
       </c>
       <c r="D26">
         <v>13</v>
@@ -2160,10 +2160,10 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
         <v>92</v>
-      </c>
-      <c r="C27" t="s">
-        <v>93</v>
       </c>
       <c r="D27">
         <v>14</v>
@@ -2178,10 +2178,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" t="s">
         <v>94</v>
-      </c>
-      <c r="C28" t="s">
-        <v>95</v>
       </c>
       <c r="D28">
         <v>14</v>
@@ -2196,10 +2196,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" t="s">
         <v>96</v>
-      </c>
-      <c r="C29" t="s">
-        <v>97</v>
       </c>
       <c r="D29">
         <v>15</v>
@@ -2214,10 +2214,10 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" t="s">
         <v>70</v>
-      </c>
-      <c r="C30" t="s">
-        <v>71</v>
       </c>
       <c r="D30">
         <v>16</v>
@@ -2232,10 +2232,10 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
         <v>73</v>
-      </c>
-      <c r="C31" t="s">
-        <v>74</v>
       </c>
       <c r="D31">
         <v>17</v>

</xml_diff>

<commit_message>
Final sin QR 17 Junio
</commit_message>
<xml_diff>
--- a/CarreraObsGenerador.xlsx
+++ b/CarreraObsGenerador.xlsx
@@ -532,7 +532,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -540,17 +540,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -835,7 +853,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="A1:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,30 +866,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>97</v>
       </c>
       <c r="E2" t="str">
@@ -880,16 +898,16 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>113</v>
       </c>
       <c r="E3" t="str">
@@ -906,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="A1:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -924,54 +942,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="5" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I2" t="str">
@@ -980,28 +998,28 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="5" t="s">
         <v>100</v>
       </c>
       <c r="I3" t="str">
@@ -1023,7 +1041,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:H21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1680,8 +1700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>